<commit_message>
adding files before tagging v1
</commit_message>
<xml_diff>
--- a/docs/cs_to_graviton_pin_mapping.xlsx
+++ b/docs/cs_to_graviton_pin_mapping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16875" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="16875"/>
   </bookViews>
   <sheets>
     <sheet name="graviton_j1_to_cs_j3" sheetId="1" r:id="rId1"/>
@@ -2842,8 +2842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R380"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="R264" sqref="A233:R264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2860,7 +2860,7 @@
     <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>175</v>
       </c>
@@ -2906,99 +2906,107 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="8" t="s">
         <v>464</v>
       </c>
-      <c r="I2" t="s">
-        <v>463</v>
-      </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" t="s">
-        <v>318</v>
-      </c>
-      <c r="O2">
+      <c r="I2" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="J2" s="9">
+        <v>2</v>
+      </c>
+      <c r="K2" s="9">
+        <v>2</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9">
         <f t="shared" ref="O2:O65" si="0">IF(J2=C2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q2">
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9">
         <f t="shared" ref="Q2:Q65" si="1">IF(OR(H2=A2,RIGHT(H2,2)=RIGHT(A2,2)),1,0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="R2" s="9"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="I3" t="s">
-        <v>463</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" t="s">
-        <v>318</v>
-      </c>
-      <c r="O3">
+      <c r="I3" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="J3" s="9">
+        <v>3</v>
+      </c>
+      <c r="K3" s="9">
+        <v>3</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q3">
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="9"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>175</v>
       </c>
@@ -3044,7 +3052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>99</v>
       </c>
@@ -3090,7 +3098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>100</v>
       </c>
@@ -3136,7 +3144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>175</v>
       </c>
@@ -3182,7 +3190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>101</v>
       </c>
@@ -3228,7 +3236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
@@ -3274,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>175</v>
       </c>
@@ -3320,7 +3328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>175</v>
       </c>
@@ -3366,7 +3374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>103</v>
       </c>
@@ -3412,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>104</v>
       </c>
@@ -3458,7 +3466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>175</v>
       </c>
@@ -3504,7 +3512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>105</v>
       </c>
@@ -3550,7 +3558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
@@ -6522,7 +6530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>175</v>
       </c>
@@ -6568,99 +6576,107 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B82" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82">
+      <c r="B82" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="9">
         <v>82</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="9">
         <v>82</v>
       </c>
-      <c r="E82" t="s">
-        <v>2</v>
-      </c>
-      <c r="F82" t="s">
-        <v>3</v>
-      </c>
-      <c r="H82" s="1" t="s">
+      <c r="E82" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G82" s="9"/>
+      <c r="H82" s="8" t="s">
         <v>512</v>
       </c>
-      <c r="I82" t="s">
-        <v>463</v>
-      </c>
-      <c r="J82">
+      <c r="I82" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="J82" s="9">
         <v>82</v>
       </c>
-      <c r="K82">
+      <c r="K82" s="9">
         <v>82</v>
       </c>
-      <c r="L82" t="s">
-        <v>2</v>
-      </c>
-      <c r="M82" t="s">
-        <v>318</v>
-      </c>
-      <c r="O82">
+      <c r="L82" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M82" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="N82" s="9"/>
+      <c r="O82" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="Q82">
+      <c r="P82" s="9"/>
+      <c r="Q82" s="9">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="R82" s="9"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B83" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83">
+      <c r="B83" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" s="9">
         <v>83</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="9">
         <v>83</v>
       </c>
-      <c r="E83" t="s">
-        <v>2</v>
-      </c>
-      <c r="F83" t="s">
-        <v>3</v>
-      </c>
-      <c r="H83" s="1" t="s">
+      <c r="E83" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G83" s="9"/>
+      <c r="H83" s="8" t="s">
         <v>513</v>
       </c>
-      <c r="I83" t="s">
-        <v>463</v>
-      </c>
-      <c r="J83">
+      <c r="I83" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="J83" s="9">
         <v>83</v>
       </c>
-      <c r="K83">
+      <c r="K83" s="9">
         <v>83</v>
       </c>
-      <c r="L83" t="s">
-        <v>2</v>
-      </c>
-      <c r="M83" t="s">
-        <v>318</v>
-      </c>
-      <c r="O83">
+      <c r="L83" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M83" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="N83" s="9"/>
+      <c r="O83" s="9">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="Q83">
+      <c r="P83" s="9"/>
+      <c r="Q83" s="9">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R83" s="9"/>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>175</v>
       </c>
@@ -6706,7 +6722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>78</v>
       </c>
@@ -6752,7 +6768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>77</v>
       </c>
@@ -6798,7 +6814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>175</v>
       </c>
@@ -6844,7 +6860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>85</v>
       </c>
@@ -6890,7 +6906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>95</v>
       </c>
@@ -6936,7 +6952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>175</v>
       </c>
@@ -6982,7 +6998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>175</v>
       </c>
@@ -7028,7 +7044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>80</v>
       </c>
@@ -7074,7 +7090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>86</v>
       </c>
@@ -7120,7 +7136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>175</v>
       </c>
@@ -7166,7 +7182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>82</v>
       </c>
@@ -7212,7 +7228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>88</v>
       </c>
@@ -14195,7 +14211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A257" s="8" t="s">
         <v>167</v>
       </c>
@@ -14244,7 +14260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>175</v>
       </c>
@@ -14290,7 +14306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A259" s="8" t="s">
         <v>155</v>
       </c>
@@ -14339,7 +14355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A260" s="8" t="s">
         <v>154</v>
       </c>
@@ -14388,7 +14404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>175</v>
       </c>
@@ -14434,7 +14450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>175</v>
       </c>
@@ -14480,99 +14496,107 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A263" s="1" t="s">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A263" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B263" t="s">
-        <v>1</v>
-      </c>
-      <c r="C263">
+      <c r="B263" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C263" s="9">
         <v>282</v>
       </c>
-      <c r="D263">
+      <c r="D263" s="9">
         <v>282</v>
       </c>
-      <c r="E263" t="s">
-        <v>2</v>
-      </c>
-      <c r="F263" t="s">
-        <v>3</v>
-      </c>
-      <c r="H263" s="1" t="s">
+      <c r="E263" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F263" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G263" s="9"/>
+      <c r="H263" s="8" t="s">
         <v>576</v>
       </c>
-      <c r="I263" t="s">
-        <v>463</v>
-      </c>
-      <c r="J263">
+      <c r="I263" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="J263" s="9">
         <v>282</v>
       </c>
-      <c r="K263">
+      <c r="K263" s="9">
         <v>282</v>
       </c>
-      <c r="L263" t="s">
-        <v>2</v>
-      </c>
-      <c r="M263" t="s">
-        <v>318</v>
-      </c>
-      <c r="O263">
+      <c r="L263" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M263" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="N263" s="9"/>
+      <c r="O263" s="9">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="Q263">
+      <c r="P263" s="9"/>
+      <c r="Q263" s="9">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A264" s="1" t="s">
+      <c r="R263" s="9"/>
+    </row>
+    <row r="264" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A264" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B264" t="s">
-        <v>1</v>
-      </c>
-      <c r="C264">
+      <c r="B264" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C264" s="9">
         <v>283</v>
       </c>
-      <c r="D264">
+      <c r="D264" s="9">
         <v>283</v>
       </c>
-      <c r="E264" t="s">
-        <v>2</v>
-      </c>
-      <c r="F264" t="s">
-        <v>3</v>
-      </c>
-      <c r="H264" s="1" t="s">
+      <c r="E264" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F264" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G264" s="9"/>
+      <c r="H264" s="8" t="s">
         <v>577</v>
       </c>
-      <c r="I264" t="s">
-        <v>463</v>
-      </c>
-      <c r="J264">
+      <c r="I264" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="J264" s="9">
         <v>283</v>
       </c>
-      <c r="K264">
+      <c r="K264" s="9">
         <v>283</v>
       </c>
-      <c r="L264" t="s">
-        <v>2</v>
-      </c>
-      <c r="M264" t="s">
-        <v>318</v>
-      </c>
-      <c r="O264">
+      <c r="L264" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M264" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="N264" s="9"/>
+      <c r="O264" s="9">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="Q264">
+      <c r="P264" s="9"/>
+      <c r="Q264" s="9">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R264" s="9"/>
+    </row>
+    <row r="265" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>175</v>
       </c>
@@ -14618,7 +14642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>6</v>
       </c>
@@ -14664,7 +14688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>7</v>
       </c>
@@ -14710,7 +14734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>175</v>
       </c>
@@ -14756,7 +14780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>8</v>
       </c>
@@ -14802,7 +14826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>24</v>
       </c>
@@ -14848,7 +14872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>175</v>
       </c>
@@ -14894,7 +14918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>175</v>
       </c>
@@ -19910,8 +19934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R326"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView topLeftCell="A231" workbookViewId="0">
+      <selection activeCell="H257" sqref="H257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19928,7 +19952,7 @@
     <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>175</v>
       </c>
@@ -19974,99 +19998,107 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="C2" s="9">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="H2" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" t="s">
-        <v>318</v>
-      </c>
-      <c r="O2">
+      <c r="J2" s="9">
+        <v>2</v>
+      </c>
+      <c r="K2" s="9">
+        <v>2</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9">
         <f t="shared" ref="O2:O65" si="0">IF(J2=C2,1,0)</f>
         <v>1</v>
       </c>
-      <c r="Q2">
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9">
         <f t="shared" ref="Q2:Q65" si="1">IF(OR(H2=A2,RIGHT(H2,2)=RIGHT(A2,2)),1,0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="R2" s="9"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="C3" s="9">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" t="s">
-        <v>318</v>
-      </c>
-      <c r="O3">
+      <c r="J3" s="9">
+        <v>3</v>
+      </c>
+      <c r="K3" s="9">
+        <v>3</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q3">
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="9"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>175</v>
       </c>
@@ -20112,7 +20144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>249</v>
       </c>
@@ -20158,7 +20190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>250</v>
       </c>
@@ -20204,7 +20236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>175</v>
       </c>
@@ -20250,7 +20282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>251</v>
       </c>
@@ -20296,7 +20328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>252</v>
       </c>
@@ -20342,7 +20374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>175</v>
       </c>
@@ -20388,7 +20420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>175</v>
       </c>
@@ -20434,7 +20466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>253</v>
       </c>
@@ -20480,7 +20512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>254</v>
       </c>
@@ -20526,7 +20558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>175</v>
       </c>
@@ -20572,7 +20604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>255</v>
       </c>
@@ -20618,7 +20650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>256</v>
       </c>
@@ -31534,99 +31566,107 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A257" s="1" t="s">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A257" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B257" t="s">
+      <c r="B257" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C257">
+      <c r="C257" s="9">
         <v>282</v>
       </c>
-      <c r="D257">
+      <c r="D257" s="9">
         <v>282</v>
       </c>
-      <c r="E257" t="s">
-        <v>2</v>
-      </c>
-      <c r="F257" t="s">
-        <v>3</v>
-      </c>
-      <c r="H257" s="1" t="s">
+      <c r="E257" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F257" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G257" s="9"/>
+      <c r="H257" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="I257" t="s">
+      <c r="I257" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="J257">
+      <c r="J257" s="9">
         <v>282</v>
       </c>
-      <c r="K257">
+      <c r="K257" s="9">
         <v>282</v>
       </c>
-      <c r="L257" t="s">
-        <v>2</v>
-      </c>
-      <c r="M257" t="s">
-        <v>318</v>
-      </c>
-      <c r="O257">
+      <c r="L257" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M257" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="N257" s="9"/>
+      <c r="O257" s="9">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q257">
+      <c r="P257" s="9"/>
+      <c r="Q257" s="9">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A258" s="1" t="s">
+      <c r="R257" s="9"/>
+    </row>
+    <row r="258" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A258" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="B258" t="s">
+      <c r="B258" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C258">
+      <c r="C258" s="9">
         <v>283</v>
       </c>
-      <c r="D258">
+      <c r="D258" s="9">
         <v>283</v>
       </c>
-      <c r="E258" t="s">
-        <v>2</v>
-      </c>
-      <c r="F258" t="s">
-        <v>3</v>
-      </c>
-      <c r="H258" s="1" t="s">
+      <c r="E258" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F258" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G258" s="9"/>
+      <c r="H258" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="I258" t="s">
+      <c r="I258" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="J258">
+      <c r="J258" s="9">
         <v>283</v>
       </c>
-      <c r="K258">
+      <c r="K258" s="9">
         <v>283</v>
       </c>
-      <c r="L258" t="s">
-        <v>2</v>
-      </c>
-      <c r="M258" t="s">
-        <v>318</v>
-      </c>
-      <c r="O258">
+      <c r="L258" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M258" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="N258" s="9"/>
+      <c r="O258" s="9">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q258">
+      <c r="P258" s="9"/>
+      <c r="Q258" s="9">
         <f t="shared" ref="Q258:Q321" si="8">IF(OR(H258=A258,RIGHT(H258,2)=RIGHT(A258,2)),1,0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R258" s="9"/>
+    </row>
+    <row r="259" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>175</v>
       </c>
@@ -31672,7 +31712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>183</v>
       </c>
@@ -31718,7 +31758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>191</v>
       </c>
@@ -31764,7 +31804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>175</v>
       </c>
@@ -31810,7 +31850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>180</v>
       </c>
@@ -31856,7 +31896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>179</v>
       </c>
@@ -31902,7 +31942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>175</v>
       </c>
@@ -31948,7 +31988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>175</v>
       </c>
@@ -31994,7 +32034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>187</v>
       </c>
@@ -32040,7 +32080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>188</v>
       </c>
@@ -32086,7 +32126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>175</v>
       </c>
@@ -32132,7 +32172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>185</v>
       </c>
@@ -32178,7 +32218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>186</v>
       </c>
@@ -32224,7 +32264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>175</v>
       </c>

</xml_diff>